<commit_message>
Faza 1 - finally version
</commit_message>
<xml_diff>
--- a/Faza 1/2b Format partner budget - Horizon2020 - ETF.xlsx
+++ b/Faza 1/2b Format partner budget - Horizon2020 - ETF.xlsx
@@ -1398,10 +1398,13 @@
         <f t="shared" ref="Q14:Q22" si="2">+J14+K14+L14+M14+O14+P14</f>
         <v>186000</v>
       </c>
-      <c r="R14" s="35"/>
+      <c r="R14" s="36">
+        <f t="shared" ref="R14:R23" si="3">Q14</f>
+        <v>186000</v>
+      </c>
       <c r="S14" s="36">
-        <f t="shared" ref="S14:S22" si="3">+Q14-R14</f>
-        <v>186000</v>
+        <f t="shared" ref="S14:S22" si="4">+Q14-R14</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
@@ -1435,7 +1438,7 @@
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
       <c r="O15" s="35">
-        <f t="shared" ref="O15:O22" si="4">+$O$4*(J15+K15-N15)</f>
+        <f t="shared" ref="O15:O22" si="5">+$O$4*(J15+K15-N15)</f>
         <v>3750</v>
       </c>
       <c r="P15" s="34"/>
@@ -1443,10 +1446,13 @@
         <f t="shared" si="2"/>
         <v>18750</v>
       </c>
-      <c r="R15" s="35"/>
-      <c r="S15" s="36">
+      <c r="R15" s="36">
         <f t="shared" si="3"/>
         <v>18750</v>
+      </c>
+      <c r="S15" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -1478,7 +1484,7 @@
       <c r="M16" s="34"/>
       <c r="N16" s="34"/>
       <c r="O16" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3375</v>
       </c>
       <c r="P16" s="34"/>
@@ -1486,10 +1492,13 @@
         <f t="shared" si="2"/>
         <v>16875</v>
       </c>
-      <c r="R16" s="35"/>
-      <c r="S16" s="36">
+      <c r="R16" s="36">
         <f t="shared" si="3"/>
         <v>16875</v>
+      </c>
+      <c r="S16" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1513,7 +1522,7 @@
       <c r="M17" s="34"/>
       <c r="N17" s="34"/>
       <c r="O17" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P17" s="34"/>
@@ -1521,9 +1530,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R17" s="35"/>
+      <c r="R17" s="36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="S17" s="36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1554,7 +1566,7 @@
       <c r="M18" s="34"/>
       <c r="N18" s="34"/>
       <c r="O18" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2750</v>
       </c>
       <c r="P18" s="34"/>
@@ -1562,10 +1574,13 @@
         <f t="shared" si="2"/>
         <v>13750</v>
       </c>
-      <c r="R18" s="35"/>
-      <c r="S18" s="36">
+      <c r="R18" s="36">
         <f t="shared" si="3"/>
         <v>13750</v>
+      </c>
+      <c r="S18" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
@@ -1591,7 +1606,7 @@
       <c r="M19" s="34"/>
       <c r="N19" s="34"/>
       <c r="O19" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16000</v>
       </c>
       <c r="P19" s="34"/>
@@ -1599,10 +1614,13 @@
         <f t="shared" si="2"/>
         <v>80000</v>
       </c>
-      <c r="R19" s="35"/>
-      <c r="S19" s="36">
+      <c r="R19" s="36">
         <f t="shared" si="3"/>
         <v>80000</v>
+      </c>
+      <c r="S19" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1636,7 +1654,7 @@
       <c r="M20" s="34"/>
       <c r="N20" s="34"/>
       <c r="O20" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4500</v>
       </c>
       <c r="P20" s="34"/>
@@ -1644,10 +1662,13 @@
         <f t="shared" si="2"/>
         <v>22500</v>
       </c>
-      <c r="R20" s="35"/>
-      <c r="S20" s="36">
+      <c r="R20" s="36">
         <f t="shared" si="3"/>
         <v>22500</v>
+      </c>
+      <c r="S20" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
@@ -1683,7 +1704,7 @@
       <c r="M21" s="34"/>
       <c r="N21" s="34"/>
       <c r="O21" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9000</v>
       </c>
       <c r="P21" s="34"/>
@@ -1691,10 +1712,13 @@
         <f t="shared" si="2"/>
         <v>70000</v>
       </c>
-      <c r="R21" s="35"/>
-      <c r="S21" s="36">
+      <c r="R21" s="36">
         <f t="shared" si="3"/>
         <v>70000</v>
+      </c>
+      <c r="S21" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
@@ -1728,7 +1752,7 @@
       <c r="M22" s="34"/>
       <c r="N22" s="34"/>
       <c r="O22" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8250</v>
       </c>
       <c r="P22" s="34"/>
@@ -1736,10 +1760,13 @@
         <f t="shared" si="2"/>
         <v>41250</v>
       </c>
-      <c r="R22" s="35"/>
-      <c r="S22" s="36">
+      <c r="R22" s="36">
         <f t="shared" si="3"/>
         <v>41250</v>
+      </c>
+      <c r="S22" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1775,7 +1802,10 @@
       <c r="O23" s="35"/>
       <c r="P23" s="34"/>
       <c r="Q23" s="34"/>
-      <c r="R23" s="35"/>
+      <c r="R23" s="36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="S23" s="35"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
@@ -1890,68 +1920,68 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="37">
-        <f t="shared" ref="D27:S27" si="5">SUM(D14:D26)</f>
+        <f t="shared" ref="D27:S27" si="6">SUM(D14:D26)</f>
         <v>22</v>
       </c>
       <c r="E27" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="F27" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>63</v>
       </c>
       <c r="G27" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H27" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
       <c r="I27" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>129</v>
       </c>
       <c r="J27" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>205500</v>
       </c>
       <c r="K27" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>156000</v>
       </c>
       <c r="L27" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>76000</v>
       </c>
       <c r="M27" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10000</v>
       </c>
       <c r="N27" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O27" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>74625</v>
       </c>
       <c r="P27" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q27" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>449125</v>
       </c>
       <c r="R27" s="42">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>449125</v>
       </c>
       <c r="S27" s="43">
-        <f t="shared" si="5"/>
-        <v>449125</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="T27" s="44"/>
     </row>

</xml_diff>